<commit_message>
Modifications to Chef's SlideRule
</commit_message>
<xml_diff>
--- a/ChefsSliderule/icon/fractions.xlsx
+++ b/ChefsSliderule/icon/fractions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>¼</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>\u215E</t>
+  </si>
+  <si>
+    <t>Unicode</t>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
   </si>
 </sst>
 </file>
@@ -401,218 +416,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C1">
+      <c r="C2">
+        <v>0.125</v>
+      </c>
+      <c r="D2">
+        <v>6.2E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+      <c r="D3">
+        <v>0.188</v>
+      </c>
+      <c r="E3">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0.375</v>
+      </c>
+      <c r="D5">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.438</v>
+      </c>
+      <c r="E6">
+        <v>0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>0.625</v>
+      </c>
+      <c r="D7">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="E7">
+        <v>0.64600000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D8">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="E8">
+        <v>0.70899999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>0.75</v>
+      </c>
+      <c r="D9">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="E9">
+        <v>0.81299999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="E1">
-        <v>0.125</v>
-      </c>
-      <c r="F1">
-        <v>6.2E-2</v>
-      </c>
-      <c r="G1">
-        <v>0.188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>0.25</v>
-      </c>
-      <c r="F2">
-        <v>0.188</v>
-      </c>
-      <c r="G2">
-        <v>0.29199999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="F3">
-        <v>0.29199999999999998</v>
-      </c>
-      <c r="G3">
-        <v>0.35399999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>0.375</v>
-      </c>
-      <c r="F4">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="G4">
-        <v>0.438</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>0.5</v>
-      </c>
-      <c r="F5">
-        <v>0.438</v>
-      </c>
-      <c r="G5">
-        <v>0.56299999999999994</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>0.625</v>
-      </c>
-      <c r="F6">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="G6">
-        <v>0.64600000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="F7">
-        <v>0.64600000000000002</v>
-      </c>
-      <c r="G7">
-        <v>0.70899999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>0.75</v>
-      </c>
-      <c r="F8">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="G8">
+      <c r="C10">
+        <v>0.875</v>
+      </c>
+      <c r="D10">
         <v>0.81299999999999994</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
-        <v>0.875</v>
-      </c>
-      <c r="F9">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="G9">
+      <c r="E10">
         <v>0.94799999999999995</v>
       </c>
     </row>

</xml_diff>